<commit_message>
Fixed caps issue on ORF
</commit_message>
<xml_diff>
--- a/reference/Peach_Rules_12232021_FINAL.xlsx
+++ b/reference/Peach_Rules_12232021_FINAL.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinav/Desktop/SEMA4/Rules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremymiller/PycharmProjects/AtriumBCCGeneWeb/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66ECB970-83D8-C34B-A1AA-BCBEC815AFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D6A75C-16AC-8349-BA1B-2F4B9E1EB86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="rules as of today" sheetId="1" r:id="rId1"/>
+    <sheet name="Main" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'rules as of today'!$A$1:$G$689</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$G$689</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3003,7 +3003,7 @@
   <dimension ref="A1:G709"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="J127" sqref="J127"/>
+      <selection activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>